<commit_message>
Fix: risolto problema di generazione grafici e migliorata compatibilità CSS
</commit_message>
<xml_diff>
--- a/Data source/Risposte_RAW.xlsx
+++ b/Data source/Risposte_RAW.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\Projects\Bike2Work\Data source\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43205561-1E0E-4321-936A-DA8EA30B7344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Risposte del modulo 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Risposte del modulo 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="376">
   <si>
     <t>Informazioni cronologiche</t>
   </si>
@@ -1120,24 +1111,53 @@
   </si>
   <si>
     <t>nn</t>
+  </si>
+  <si>
+    <t>Gli orari dei mezzi pubblici non sono compatibili con le mie esigenze, Non c'è una linea diretta / sono costretto a cambiare mezzo, La fermata di arrivo è troppo lontana dalla mia destinazione, Il mezzo pubblico non è puntuale / ci mette troppo tempo, In auto sono più comodo / ci metto meno tempo</t>
+  </si>
+  <si>
+    <t>Per evitare l'uso dell' automobile,ci dovrebbero essere più mezzi pubblici in ogni orario per riuscire ad arrivare al lavoro,inoltre se mi sposto col mezzo pubblico,dalla stazione di Lugo non c'è nessun mezzo pubblico che mi porta alla mia sede di lavoro.</t>
+  </si>
+  <si>
+    <t>Se ci fossero maggiori informazioni sui servizi / linee di trasporto pubblico</t>
+  </si>
+  <si>
+    <t>Se ci fossero bici pubbliche gratuite</t>
+  </si>
+  <si>
+    <t>Più rastrelliere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Più posti biciclette in caserma </t>
+  </si>
+  <si>
+    <t>Se gli orari dei mezzi pubblici fossero compatibili con le mie esigenze, Se ci fossero linee che mi portano a destinazione, Se la fermata fosse più vicina a casa mia, Se il mezzo pubblico fosse più puntuale, Se dovessi pagare la sosta per l'automobile</t>
+  </si>
+  <si>
+    <t>Se per gli spostamenti di lavoro si potessero usare mezzi forniti dall'Amministrazione</t>
+  </si>
+  <si>
+    <t>Economicità, Rispetto dell'ambiente, Muovermi rapidamente, Maggior libertà negli spostamenti giornalieri, Abitudine</t>
+  </si>
+  <si>
+    <t>Amplierei la zona parcheggio bici.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -1148,17 +1168,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="11">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF442F65"/>
@@ -1172,7 +1186,6 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1187,7 +1200,6 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1202,7 +1214,6 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1217,7 +1228,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1232,7 +1242,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1247,7 +1256,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1262,7 +1270,6 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1277,7 +1284,6 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1292,7 +1298,6 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1307,165 +1312,175 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF5B3F86"/>
+          <bgColor rgb="FF5B3F86"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
           <bgColor rgb="FFF8F9FA"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF5B3F86"/>
-          <bgColor rgb="FF5B3F86"/>
-        </patternFill>
-      </fill>
+      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Risposte del modulo 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    <tableStyle count="3" pivot="0" name="Risposte del modulo 1-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BG122" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:BG130" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="59">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column27"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Column28"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Column29"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Column30"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Column31"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Column32"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Column33"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Column34"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Column35"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Column36"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Column37"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Column38"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Column39"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Column40"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Column41"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Column42"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Column43"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Column44"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Column45"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Column46"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Column47"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Column48"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Column49"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Column50"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Column51"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Column52"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Column53"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Column54"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="Column55"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="Column56"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="Column57"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="Column58"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="Column59"/>
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+    <tableColumn name="Column11" id="11"/>
+    <tableColumn name="Column12" id="12"/>
+    <tableColumn name="Column13" id="13"/>
+    <tableColumn name="Column14" id="14"/>
+    <tableColumn name="Column15" id="15"/>
+    <tableColumn name="Column16" id="16"/>
+    <tableColumn name="Column17" id="17"/>
+    <tableColumn name="Column18" id="18"/>
+    <tableColumn name="Column19" id="19"/>
+    <tableColumn name="Column20" id="20"/>
+    <tableColumn name="Column21" id="21"/>
+    <tableColumn name="Column22" id="22"/>
+    <tableColumn name="Column23" id="23"/>
+    <tableColumn name="Column24" id="24"/>
+    <tableColumn name="Column25" id="25"/>
+    <tableColumn name="Column26" id="26"/>
+    <tableColumn name="Column27" id="27"/>
+    <tableColumn name="Column28" id="28"/>
+    <tableColumn name="Column29" id="29"/>
+    <tableColumn name="Column30" id="30"/>
+    <tableColumn name="Column31" id="31"/>
+    <tableColumn name="Column32" id="32"/>
+    <tableColumn name="Column33" id="33"/>
+    <tableColumn name="Column34" id="34"/>
+    <tableColumn name="Column35" id="35"/>
+    <tableColumn name="Column36" id="36"/>
+    <tableColumn name="Column37" id="37"/>
+    <tableColumn name="Column38" id="38"/>
+    <tableColumn name="Column39" id="39"/>
+    <tableColumn name="Column40" id="40"/>
+    <tableColumn name="Column41" id="41"/>
+    <tableColumn name="Column42" id="42"/>
+    <tableColumn name="Column43" id="43"/>
+    <tableColumn name="Column44" id="44"/>
+    <tableColumn name="Column45" id="45"/>
+    <tableColumn name="Column46" id="46"/>
+    <tableColumn name="Column47" id="47"/>
+    <tableColumn name="Column48" id="48"/>
+    <tableColumn name="Column49" id="49"/>
+    <tableColumn name="Column50" id="50"/>
+    <tableColumn name="Column51" id="51"/>
+    <tableColumn name="Column52" id="52"/>
+    <tableColumn name="Column53" id="53"/>
+    <tableColumn name="Column54" id="54"/>
+    <tableColumn name="Column55" id="55"/>
+    <tableColumn name="Column56" id="56"/>
+    <tableColumn name="Column57" id="57"/>
+    <tableColumn name="Column58" id="58"/>
+    <tableColumn name="Column59" id="59"/>
   </tableColumns>
-  <tableStyleInfo name="Risposte del modulo 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Risposte del modulo 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -1475,7 +1490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1665,86 +1680,83 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1:V1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.90625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" customWidth="1"/>
-    <col min="4" max="4" width="26.90625" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" customWidth="1"/>
-    <col min="6" max="6" width="19.90625" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.90625" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="25.90625" customWidth="1"/>
-    <col min="11" max="11" width="24.26953125" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
-    <col min="13" max="13" width="24.90625" customWidth="1"/>
-    <col min="14" max="14" width="31.453125" customWidth="1"/>
-    <col min="15" max="15" width="29.453125" customWidth="1"/>
-    <col min="16" max="16" width="26.453125" customWidth="1"/>
-    <col min="17" max="17" width="46.36328125" customWidth="1"/>
-    <col min="18" max="18" width="23.90625" customWidth="1"/>
-    <col min="19" max="19" width="44" customWidth="1"/>
-    <col min="20" max="20" width="254.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="87.7265625" customWidth="1"/>
-    <col min="22" max="22" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.36328125" customWidth="1"/>
-    <col min="24" max="24" width="46.90625" customWidth="1"/>
-    <col min="25" max="25" width="69.6328125" customWidth="1"/>
-    <col min="26" max="26" width="54.90625" customWidth="1"/>
-    <col min="27" max="27" width="38.26953125" customWidth="1"/>
-    <col min="28" max="28" width="57.08984375" customWidth="1"/>
-    <col min="29" max="29" width="56.90625" customWidth="1"/>
-    <col min="30" max="30" width="107.6328125" customWidth="1"/>
-    <col min="31" max="32" width="53.36328125" customWidth="1"/>
-    <col min="33" max="33" width="61.36328125" customWidth="1"/>
-    <col min="34" max="34" width="81.7265625" customWidth="1"/>
-    <col min="35" max="35" width="61.36328125" customWidth="1"/>
-    <col min="36" max="36" width="81.7265625" customWidth="1"/>
-    <col min="37" max="37" width="60.36328125" customWidth="1"/>
-    <col min="38" max="38" width="61" customWidth="1"/>
-    <col min="39" max="39" width="27.90625" customWidth="1"/>
-    <col min="40" max="40" width="38" customWidth="1"/>
-    <col min="41" max="41" width="60.36328125" customWidth="1"/>
-    <col min="42" max="42" width="61.36328125" customWidth="1"/>
-    <col min="43" max="43" width="81.7265625" customWidth="1"/>
-    <col min="44" max="44" width="49.453125" customWidth="1"/>
-    <col min="45" max="45" width="27.90625" customWidth="1"/>
-    <col min="46" max="46" width="60.36328125" customWidth="1"/>
-    <col min="47" max="47" width="61" customWidth="1"/>
-    <col min="48" max="48" width="27.90625" customWidth="1"/>
-    <col min="49" max="49" width="38" customWidth="1"/>
-    <col min="50" max="51" width="133.7265625" customWidth="1"/>
-    <col min="52" max="52" width="52" customWidth="1"/>
-    <col min="53" max="53" width="68.453125" customWidth="1"/>
-    <col min="54" max="54" width="52" customWidth="1"/>
-    <col min="55" max="55" width="124" customWidth="1"/>
-    <col min="56" max="56" width="62.7265625" customWidth="1"/>
-    <col min="57" max="57" width="448.36328125" customWidth="1"/>
-    <col min="58" max="58" width="68.08984375" customWidth="1"/>
-    <col min="59" max="59" width="27.90625" customWidth="1"/>
-    <col min="60" max="65" width="18.90625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="24.88"/>
+    <col customWidth="1" min="2" max="2" width="10.0"/>
+    <col customWidth="1" min="3" max="3" width="7.88"/>
+    <col customWidth="1" min="4" max="4" width="26.88"/>
+    <col customWidth="1" min="5" max="5" width="21.5"/>
+    <col customWidth="1" min="6" max="6" width="19.88"/>
+    <col customWidth="1" min="7" max="7" width="20.5"/>
+    <col customWidth="1" min="8" max="8" width="18.88"/>
+    <col customWidth="1" min="9" max="9" width="27.0"/>
+    <col customWidth="1" min="10" max="10" width="25.88"/>
+    <col customWidth="1" min="11" max="11" width="24.25"/>
+    <col customWidth="1" min="12" max="12" width="23.25"/>
+    <col customWidth="1" min="13" max="13" width="24.88"/>
+    <col customWidth="1" min="14" max="14" width="31.5"/>
+    <col customWidth="1" min="15" max="15" width="29.5"/>
+    <col customWidth="1" min="16" max="16" width="26.5"/>
+    <col customWidth="1" min="17" max="17" width="46.38"/>
+    <col customWidth="1" min="18" max="18" width="23.88"/>
+    <col customWidth="1" min="19" max="19" width="44.0"/>
+    <col customWidth="1" min="20" max="20" width="28.88"/>
+    <col customWidth="1" min="21" max="21" width="37.38"/>
+    <col customWidth="1" min="22" max="22" width="13.88"/>
+    <col customWidth="1" min="23" max="23" width="32.38"/>
+    <col customWidth="1" min="24" max="24" width="46.88"/>
+    <col customWidth="1" min="25" max="25" width="69.63"/>
+    <col customWidth="1" min="26" max="26" width="54.88"/>
+    <col customWidth="1" min="27" max="27" width="38.25"/>
+    <col customWidth="1" min="28" max="28" width="57.13"/>
+    <col customWidth="1" min="29" max="29" width="56.88"/>
+    <col customWidth="1" min="30" max="30" width="107.63"/>
+    <col customWidth="1" min="31" max="32" width="53.38"/>
+    <col customWidth="1" min="33" max="33" width="61.38"/>
+    <col customWidth="1" min="34" max="34" width="81.75"/>
+    <col customWidth="1" min="35" max="35" width="61.38"/>
+    <col customWidth="1" min="36" max="36" width="81.75"/>
+    <col customWidth="1" min="37" max="37" width="60.38"/>
+    <col customWidth="1" min="38" max="38" width="61.0"/>
+    <col customWidth="1" min="39" max="39" width="27.88"/>
+    <col customWidth="1" min="40" max="40" width="38.0"/>
+    <col customWidth="1" min="41" max="41" width="60.38"/>
+    <col customWidth="1" min="42" max="42" width="61.38"/>
+    <col customWidth="1" min="43" max="43" width="81.75"/>
+    <col customWidth="1" min="44" max="44" width="49.5"/>
+    <col customWidth="1" min="45" max="45" width="27.88"/>
+    <col customWidth="1" min="46" max="46" width="60.38"/>
+    <col customWidth="1" min="47" max="47" width="61.0"/>
+    <col customWidth="1" min="48" max="48" width="27.88"/>
+    <col customWidth="1" min="49" max="49" width="38.0"/>
+    <col customWidth="1" min="50" max="51" width="133.75"/>
+    <col customWidth="1" min="52" max="52" width="52.0"/>
+    <col customWidth="1" min="53" max="53" width="68.5"/>
+    <col customWidth="1" min="54" max="54" width="52.0"/>
+    <col customWidth="1" min="55" max="55" width="124.0"/>
+    <col customWidth="1" min="56" max="56" width="62.75"/>
+    <col customWidth="1" min="57" max="57" width="448.38"/>
+    <col customWidth="1" min="58" max="58" width="68.13"/>
+    <col customWidth="1" min="59" max="59" width="27.88"/>
+    <col customWidth="1" min="60" max="65" width="18.88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1923,9 +1935,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="4">
-        <v>45804.616113206022</v>
+        <v>45804.61611320602</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>45</v>
@@ -2028,7 +2040,7 @@
         <v>68</v>
       </c>
       <c r="BB2" s="5">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC2" s="5" t="s">
         <v>69</v>
@@ -2042,9 +2054,9 @@
       <c r="BF2" s="6"/>
       <c r="BG2" s="7"/>
     </row>
-    <row r="3" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="8">
-        <v>45804.616531342588</v>
+        <v>45804.61653134259</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>45</v>
@@ -2119,7 +2131,7 @@
         <v>81</v>
       </c>
       <c r="BB3" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC3" s="9" t="s">
         <v>82</v>
@@ -2128,9 +2140,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="10">
-        <v>45804.635733726856</v>
+        <v>45804.63573372686</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>45</v>
@@ -2205,7 +2217,7 @@
         <v>87</v>
       </c>
       <c r="BB4" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC4" s="11" t="s">
         <v>88</v>
@@ -2214,9 +2226,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="8">
-        <v>45804.652549270832</v>
+        <v>45804.65254927083</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>45</v>
@@ -2276,15 +2288,15 @@
         <v>95</v>
       </c>
       <c r="AJ5" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ5" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="10">
-        <v>45804.722113009258</v>
+        <v>45804.72211300926</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>45</v>
@@ -2344,15 +2356,15 @@
         <v>99</v>
       </c>
       <c r="AJ6" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ6" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="8">
-        <v>45804.778981631942</v>
+        <v>45804.77898163194</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>45</v>
@@ -2415,16 +2427,16 @@
         <v>103</v>
       </c>
       <c r="AJ7" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ7" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE7" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="10">
         <v>45805.38386155093</v>
       </c>
@@ -2501,7 +2513,7 @@
         <v>112</v>
       </c>
       <c r="BB8" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC8" s="11" t="s">
         <v>113</v>
@@ -2510,7 +2522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="8">
         <v>45805.391008032406</v>
       </c>
@@ -2572,15 +2584,15 @@
         <v>116</v>
       </c>
       <c r="AJ9" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ9" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="10">
-        <v>45805.400433252318</v>
+        <v>45805.40043325232</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>45</v>
@@ -2640,13 +2652,13 @@
         <v>117</v>
       </c>
       <c r="AJ10" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ10" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="8">
         <v>45805.412378587964</v>
       </c>
@@ -2708,15 +2720,15 @@
         <v>124</v>
       </c>
       <c r="AQ11" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ11" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="10">
-        <v>45805.442984502311</v>
+        <v>45805.44298450231</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>45</v>
@@ -2776,16 +2788,16 @@
         <v>133</v>
       </c>
       <c r="AH12" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ12" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE12" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="8">
         <v>45805.447943136576</v>
       </c>
@@ -2862,7 +2874,7 @@
         <v>139</v>
       </c>
       <c r="BB13" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC13" s="9" t="s">
         <v>140</v>
@@ -2874,9 +2886,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="10">
-        <v>45805.454951979162</v>
+        <v>45805.45495197916</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>45</v>
@@ -2948,7 +2960,7 @@
         <v>68</v>
       </c>
       <c r="BB14" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC14" s="11" t="s">
         <v>89</v>
@@ -2960,7 +2972,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="8">
         <v>45805.642305243055</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>68</v>
       </c>
       <c r="BB15" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC15" s="9" t="s">
         <v>148</v>
@@ -3043,9 +3055,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="10">
-        <v>45805.642335405093</v>
+        <v>45805.64233540509</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>45</v>
@@ -3117,7 +3129,7 @@
         <v>68</v>
       </c>
       <c r="BB16" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC16" s="11" t="s">
         <v>150</v>
@@ -3126,7 +3138,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="8">
         <v>45805.642463634256</v>
       </c>
@@ -3200,7 +3212,7 @@
         <v>155</v>
       </c>
       <c r="BB17" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC17" s="9" t="s">
         <v>156</v>
@@ -3209,7 +3221,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="10">
         <v>45805.64350288194</v>
       </c>
@@ -3286,18 +3298,18 @@
         <v>161</v>
       </c>
       <c r="AQ18" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY18" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ18" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="8">
-        <v>45805.643725868053</v>
+        <v>45805.64372586805</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>45</v>
@@ -3369,7 +3381,7 @@
         <v>165</v>
       </c>
       <c r="BB19" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC19" s="9" t="s">
         <v>166</v>
@@ -3378,9 +3390,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="10">
-        <v>45805.644398287041</v>
+        <v>45805.64439828704</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>45</v>
@@ -3452,7 +3464,7 @@
         <v>68</v>
       </c>
       <c r="BB20" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC20" s="11" t="s">
         <v>88</v>
@@ -3461,9 +3473,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="8">
-        <v>45805.645077557871</v>
+        <v>45805.64507755787</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>45</v>
@@ -3535,7 +3547,7 @@
         <v>173</v>
       </c>
       <c r="BB21" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC21" s="9" t="s">
         <v>88</v>
@@ -3547,9 +3559,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="10">
-        <v>45805.645573009257</v>
+        <v>45805.64557300926</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>45</v>
@@ -3621,7 +3633,7 @@
         <v>178</v>
       </c>
       <c r="BB22" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC22" s="11" t="s">
         <v>166</v>
@@ -3633,7 +3645,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="8">
         <v>45805.64634388889</v>
       </c>
@@ -3707,7 +3719,7 @@
         <v>183</v>
       </c>
       <c r="BB23" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC23" s="9" t="s">
         <v>166</v>
@@ -3716,9 +3728,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="10">
-        <v>45805.646880289351</v>
+        <v>45805.64688028935</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>45</v>
@@ -3790,7 +3802,7 @@
         <v>68</v>
       </c>
       <c r="BB24" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC24" s="11" t="s">
         <v>166</v>
@@ -3799,9 +3811,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="8">
-        <v>45805.647149432873</v>
+        <v>45805.64714943287</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>45</v>
@@ -3873,7 +3885,7 @@
         <v>186</v>
       </c>
       <c r="BB25" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC25" s="9" t="s">
         <v>166</v>
@@ -3882,7 +3894,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="10">
         <v>45805.647847175926</v>
       </c>
@@ -3947,13 +3959,13 @@
         <v>190</v>
       </c>
       <c r="AQ26" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ26" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" s="8">
         <v>45805.649957013884</v>
       </c>
@@ -4027,7 +4039,7 @@
         <v>68</v>
       </c>
       <c r="BB27" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC27" s="9" t="s">
         <v>166</v>
@@ -4036,7 +4048,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="10">
         <v>45805.65057456019</v>
       </c>
@@ -4113,7 +4125,7 @@
         <v>68</v>
       </c>
       <c r="BB28" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC28" s="11" t="s">
         <v>69</v>
@@ -4122,7 +4134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="8">
         <v>45805.651052615736</v>
       </c>
@@ -4196,7 +4208,7 @@
         <v>68</v>
       </c>
       <c r="BB29" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC29" s="9" t="s">
         <v>166</v>
@@ -4205,7 +4217,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="10">
         <v>45805.656936747684</v>
       </c>
@@ -4282,7 +4294,7 @@
         <v>194</v>
       </c>
       <c r="BB30" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC30" s="11" t="s">
         <v>69</v>
@@ -4294,9 +4306,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="8">
-        <v>45805.657394247683</v>
+        <v>45805.65739424768</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>45</v>
@@ -4371,7 +4383,7 @@
         <v>68</v>
       </c>
       <c r="BB31" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC31" s="9" t="s">
         <v>69</v>
@@ -4380,7 +4392,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" s="10">
         <v>45805.65963944445</v>
       </c>
@@ -4457,7 +4469,7 @@
         <v>68</v>
       </c>
       <c r="BB32" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC32" s="11" t="s">
         <v>69</v>
@@ -4466,9 +4478,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" s="8">
-        <v>45805.879857152773</v>
+        <v>45805.87985715277</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>45</v>
@@ -4528,18 +4540,18 @@
         <v>199</v>
       </c>
       <c r="AJ33" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ33" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE33" s="9" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" s="10">
-        <v>45806.306799849539</v>
+        <v>45806.30679984954</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>45</v>
@@ -4599,13 +4611,13 @@
         <v>203</v>
       </c>
       <c r="AJ34" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ34" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="8">
         <v>45806.31661248843</v>
       </c>
@@ -4679,18 +4691,18 @@
         <v>206</v>
       </c>
       <c r="AQ35" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY35" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ35" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="10">
-        <v>45806.317079756947</v>
+        <v>45806.31707975695</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>45</v>
@@ -4753,15 +4765,15 @@
         <v>208</v>
       </c>
       <c r="AQ36" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ36" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="8">
-        <v>45806.319117025458</v>
+        <v>45806.31911702546</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>45</v>
@@ -4821,18 +4833,18 @@
         <v>209</v>
       </c>
       <c r="AJ37" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ37" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE37" s="9" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" s="10">
-        <v>45806.319847476851</v>
+        <v>45806.31984747685</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>45</v>
@@ -4889,10 +4901,10 @@
         <v>62</v>
       </c>
       <c r="AZ38" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="8">
         <v>45806.3203765625</v>
       </c>
@@ -4966,7 +4978,7 @@
         <v>214</v>
       </c>
       <c r="BB39" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC39" s="9" t="s">
         <v>88</v>
@@ -4978,9 +4990,9 @@
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" s="10">
-        <v>45806.320960254627</v>
+        <v>45806.32096025463</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>45</v>
@@ -5037,10 +5049,10 @@
         <v>62</v>
       </c>
       <c r="AZ40" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" s="8">
         <v>45806.322396250005</v>
       </c>
@@ -5114,16 +5126,16 @@
         <v>209</v>
       </c>
       <c r="AQ41" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AY41" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ41" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="10">
         <v>45806.32250603009</v>
       </c>
@@ -5197,18 +5209,18 @@
         <v>209</v>
       </c>
       <c r="AQ42" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY42" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ42" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="8">
-        <v>45806.326434039351</v>
+        <v>45806.32643403935</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>45</v>
@@ -5268,13 +5280,13 @@
         <v>220</v>
       </c>
       <c r="AJ43" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ43" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" s="10">
         <v>45806.32684819444</v>
       </c>
@@ -5351,18 +5363,18 @@
         <v>224</v>
       </c>
       <c r="AQ44" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AY44" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ44" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45" s="8">
-        <v>45806.329442974537</v>
+        <v>45806.32944297454</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>45</v>
@@ -5434,7 +5446,7 @@
         <v>228</v>
       </c>
       <c r="BB45" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC45" s="9" t="s">
         <v>229</v>
@@ -5446,9 +5458,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="46" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" s="10">
-        <v>45806.344806643523</v>
+        <v>45806.34480664352</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>45</v>
@@ -5517,7 +5529,7 @@
         <v>183</v>
       </c>
       <c r="BB46" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC46" s="11" t="s">
         <v>89</v>
@@ -5526,9 +5538,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" s="8">
-        <v>45806.357370509257</v>
+        <v>45806.35737050926</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>45</v>
@@ -5588,16 +5600,16 @@
         <v>234</v>
       </c>
       <c r="AQ47" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ47" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE47" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="48" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" s="10">
         <v>45806.363646620375</v>
       </c>
@@ -5671,7 +5683,7 @@
         <v>68</v>
       </c>
       <c r="BB48" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC48" s="11" t="s">
         <v>88</v>
@@ -5683,7 +5695,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="49" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" s="8">
         <v>45806.367258171296</v>
       </c>
@@ -5754,7 +5766,7 @@
         <v>239</v>
       </c>
       <c r="BB49" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC49" s="9" t="s">
         <v>166</v>
@@ -5763,7 +5775,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" s="10">
         <v>45806.370561805554</v>
       </c>
@@ -5834,16 +5846,16 @@
         <v>241</v>
       </c>
       <c r="AQ50" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY50" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ50" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="51">
       <c r="A51" s="8">
         <v>45806.37460505787</v>
       </c>
@@ -5902,12 +5914,12 @@
         <v>62</v>
       </c>
       <c r="AZ51" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52" s="10">
-        <v>45806.382743564813</v>
+        <v>45806.38274356481</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>45</v>
@@ -5976,7 +5988,7 @@
         <v>246</v>
       </c>
       <c r="BB52" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC52" s="11" t="s">
         <v>247</v>
@@ -5985,9 +5997,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53">
       <c r="A53" s="8">
-        <v>45806.384104583332</v>
+        <v>45806.38410458333</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>45</v>
@@ -6059,7 +6071,7 @@
         <v>249</v>
       </c>
       <c r="BB53" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC53" s="9" t="s">
         <v>88</v>
@@ -6068,9 +6080,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54">
       <c r="A54" s="10">
-        <v>45806.458274525459</v>
+        <v>45806.45827452546</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>45</v>
@@ -6127,18 +6139,18 @@
         <v>250</v>
       </c>
       <c r="AJ54" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ54" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE54" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55">
       <c r="A55" s="8">
-        <v>45806.482542037033</v>
+        <v>45806.48254203703</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>45</v>
@@ -6198,18 +6210,18 @@
         <v>252</v>
       </c>
       <c r="AQ55" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ55" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE55" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="56" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56">
       <c r="A56" s="10">
-        <v>45806.626333981483</v>
+        <v>45806.62633398148</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>45</v>
@@ -6272,13 +6284,13 @@
         <v>255</v>
       </c>
       <c r="AJ56" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ56" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="57">
       <c r="A57" s="8">
         <v>45806.62943184028</v>
       </c>
@@ -6352,18 +6364,18 @@
         <v>241</v>
       </c>
       <c r="AQ57" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY57" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ57" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="58">
       <c r="A58" s="10">
-        <v>45806.635006053242</v>
+        <v>45806.63500605324</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>45</v>
@@ -6432,7 +6444,7 @@
         <v>258</v>
       </c>
       <c r="BB58" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC58" s="11" t="s">
         <v>166</v>
@@ -6441,7 +6453,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59">
       <c r="A59" s="8">
         <v>45806.7239868287</v>
       </c>
@@ -6512,7 +6524,7 @@
         <v>260</v>
       </c>
       <c r="BB59" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC59" s="9" t="s">
         <v>166</v>
@@ -6521,7 +6533,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60">
       <c r="A60" s="10">
         <v>45807.017637557874</v>
       </c>
@@ -6598,7 +6610,7 @@
         <v>261</v>
       </c>
       <c r="BB60" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC60" s="11" t="s">
         <v>261</v>
@@ -6607,9 +6619,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61">
       <c r="A61" s="8">
-        <v>45807.330862164352</v>
+        <v>45807.33086216435</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>45</v>
@@ -6681,21 +6693,21 @@
         <v>209</v>
       </c>
       <c r="AQ61" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AY61" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ61" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BE61" s="9" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62">
       <c r="A62" s="10">
-        <v>45807.391382453701</v>
+        <v>45807.3913824537</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>45</v>
@@ -6752,16 +6764,16 @@
         <v>264</v>
       </c>
       <c r="AJ62" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ62" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE62" s="11" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="63">
       <c r="A63" s="8">
         <v>45807.396517500005</v>
       </c>
@@ -6832,16 +6844,16 @@
         <v>252</v>
       </c>
       <c r="AQ63" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY63" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ63" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="64">
       <c r="A64" s="10">
         <v>45807.413250983795</v>
       </c>
@@ -6912,7 +6924,7 @@
         <v>68</v>
       </c>
       <c r="BB64" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC64" s="11" t="s">
         <v>69</v>
@@ -6924,7 +6936,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="65">
       <c r="A65" s="8">
         <v>45807.559003437505</v>
       </c>
@@ -6986,15 +6998,15 @@
         <v>208</v>
       </c>
       <c r="AQ65" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ65" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="66">
       <c r="A66" s="10">
-        <v>45807.600929456021</v>
+        <v>45807.60092945602</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>45</v>
@@ -7051,15 +7063,15 @@
         <v>275</v>
       </c>
       <c r="AJ66" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AZ66" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="67">
       <c r="A67" s="8">
-        <v>45807.657051620372</v>
+        <v>45807.65705162037</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>45</v>
@@ -7116,15 +7128,15 @@
         <v>276</v>
       </c>
       <c r="AJ67" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ67" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="68">
       <c r="A68" s="10">
-        <v>45807.713392268517</v>
+        <v>45807.71339226852</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>45</v>
@@ -7193,7 +7205,7 @@
         <v>68</v>
       </c>
       <c r="BB68" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC68" s="11" t="s">
         <v>166</v>
@@ -7202,9 +7214,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="69">
       <c r="A69" s="8">
-        <v>45807.861401261573</v>
+        <v>45807.86140126157</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>45</v>
@@ -7261,15 +7273,15 @@
         <v>278</v>
       </c>
       <c r="AJ69" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ69" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="70">
       <c r="A70" s="10">
-        <v>45808.347418449077</v>
+        <v>45808.34741844908</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>279</v>
@@ -7341,7 +7353,7 @@
         <v>280</v>
       </c>
       <c r="BB70" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC70" s="11" t="s">
         <v>69</v>
@@ -7353,9 +7365,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="71" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="71">
       <c r="A71" s="8">
-        <v>45808.359268773143</v>
+        <v>45808.35926877314</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>279</v>
@@ -7427,7 +7439,7 @@
         <v>283</v>
       </c>
       <c r="BB71" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC71" s="9" t="s">
         <v>88</v>
@@ -7439,9 +7451,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="72" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="72">
       <c r="A72" s="10">
-        <v>45808.405835555561</v>
+        <v>45808.40583555556</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>45</v>
@@ -7498,16 +7510,16 @@
         <v>286</v>
       </c>
       <c r="AJ72" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ72" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE72" s="11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="73">
       <c r="A73" s="8">
         <v>45808.448864618054</v>
       </c>
@@ -7578,16 +7590,16 @@
         <v>209</v>
       </c>
       <c r="AQ73" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY73" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ73" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
       <c r="A74" s="10">
         <v>45808.542882951384</v>
       </c>
@@ -7646,15 +7658,15 @@
         <v>224</v>
       </c>
       <c r="AJ74" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ74" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="75">
       <c r="A75" s="8">
-        <v>45808.690095543978</v>
+        <v>45808.69009554398</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>45</v>
@@ -7723,7 +7735,7 @@
         <v>258</v>
       </c>
       <c r="BB75" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC75" s="9" t="s">
         <v>166</v>
@@ -7732,9 +7744,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="76">
       <c r="A76" s="10">
-        <v>45809.623305590278</v>
+        <v>45809.62330559028</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>45</v>
@@ -7791,13 +7803,13 @@
         <v>289</v>
       </c>
       <c r="AJ76" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ76" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="77">
       <c r="A77" s="8">
         <v>45810.587880439816</v>
       </c>
@@ -7868,7 +7880,7 @@
         <v>280</v>
       </c>
       <c r="BB77" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC77" s="9" t="s">
         <v>166</v>
@@ -7877,9 +7889,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="78">
       <c r="A78" s="10">
-        <v>45810.685158379631</v>
+        <v>45810.68515837963</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>45</v>
@@ -7936,15 +7948,15 @@
         <v>293</v>
       </c>
       <c r="AH78" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ78" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="79">
       <c r="A79" s="8">
-        <v>45811.398555717591</v>
+        <v>45811.39855571759</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>45</v>
@@ -8016,7 +8028,7 @@
         <v>183</v>
       </c>
       <c r="BB79" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC79" s="9" t="s">
         <v>229</v>
@@ -8028,7 +8040,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="80" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="80">
       <c r="A80" s="10">
         <v>45811.401837314814</v>
       </c>
@@ -8102,7 +8114,7 @@
         <v>297</v>
       </c>
       <c r="BB80" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC80" s="11" t="s">
         <v>69</v>
@@ -8111,7 +8123,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="81">
       <c r="A81" s="8">
         <v>45811.53598119213</v>
       </c>
@@ -8191,7 +8203,7 @@
         <v>300</v>
       </c>
       <c r="BB81" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC81" s="9" t="s">
         <v>89</v>
@@ -8200,9 +8212,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="82" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="82">
       <c r="A82" s="10">
-        <v>45811.613637129631</v>
+        <v>45811.61363712963</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>279</v>
@@ -8274,7 +8286,7 @@
         <v>249</v>
       </c>
       <c r="BB82" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC82" s="11" t="s">
         <v>166</v>
@@ -8286,7 +8298,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="83">
       <c r="A83" s="8">
         <v>45811.61851299768</v>
       </c>
@@ -8363,16 +8375,16 @@
         <v>307</v>
       </c>
       <c r="AQ83" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AY83" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ83" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="84">
       <c r="A84" s="10">
         <v>45811.92026215278</v>
       </c>
@@ -8446,7 +8458,7 @@
         <v>68</v>
       </c>
       <c r="BB84" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC84" s="11" t="s">
         <v>69</v>
@@ -8455,7 +8467,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="85">
       <c r="A85" s="8">
         <v>45812.466701122685</v>
       </c>
@@ -8526,7 +8538,7 @@
         <v>312</v>
       </c>
       <c r="BB85" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC85" s="9" t="s">
         <v>150</v>
@@ -8535,7 +8547,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="86">
       <c r="A86" s="10">
         <v>45812.46740292824</v>
       </c>
@@ -8606,7 +8618,7 @@
         <v>314</v>
       </c>
       <c r="BB86" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC86" s="11" t="s">
         <v>166</v>
@@ -8615,7 +8627,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="87">
       <c r="A87" s="8">
         <v>45813.872885902776</v>
       </c>
@@ -8686,16 +8698,16 @@
         <v>317</v>
       </c>
       <c r="AQ87" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY87" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ87" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="88">
       <c r="A88" s="10">
         <v>45814.509593449075</v>
       </c>
@@ -8757,13 +8769,13 @@
         <v>63</v>
       </c>
       <c r="AQ88" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ88" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="89">
       <c r="A89" s="8">
         <v>45816.88691079861</v>
       </c>
@@ -8822,18 +8834,18 @@
         <v>318</v>
       </c>
       <c r="AJ89" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AZ89" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE89" s="9" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="90" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="90">
       <c r="A90" s="10">
-        <v>45817.398458900461</v>
+        <v>45817.39845890046</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>45</v>
@@ -8890,15 +8902,15 @@
         <v>252</v>
       </c>
       <c r="AJ90" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ90" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="91">
       <c r="A91" s="8">
-        <v>45817.416709120371</v>
+        <v>45817.41670912037</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>45</v>
@@ -8958,15 +8970,15 @@
         <v>278</v>
       </c>
       <c r="AQ91" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ91" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="92">
       <c r="A92" s="10">
-        <v>45818.318863159722</v>
+        <v>45818.31886315972</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>45</v>
@@ -9023,15 +9035,15 @@
         <v>321</v>
       </c>
       <c r="AJ92" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ92" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="93">
       <c r="A93" s="8">
-        <v>45818.325094861109</v>
+        <v>45818.32509486111</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>45</v>
@@ -9100,18 +9112,18 @@
         <v>323</v>
       </c>
       <c r="AQ93" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AY93" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ93" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="94">
       <c r="A94" s="10">
-        <v>45818.338627129633</v>
+        <v>45818.33862712963</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>45</v>
@@ -9171,15 +9183,15 @@
         <v>286</v>
       </c>
       <c r="AQ94" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ94" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="95">
       <c r="A95" s="8">
-        <v>45818.364386041663</v>
+        <v>45818.36438604166</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>45</v>
@@ -9251,7 +9263,7 @@
         <v>297</v>
       </c>
       <c r="BB95" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC95" s="9" t="s">
         <v>69</v>
@@ -9263,9 +9275,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="96" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="96">
       <c r="A96" s="10">
-        <v>45819.461226331019</v>
+        <v>45819.46122633102</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>45</v>
@@ -9322,15 +9334,15 @@
         <v>321</v>
       </c>
       <c r="AJ96" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ96" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="97">
       <c r="A97" s="8">
-        <v>45819.637451655093</v>
+        <v>45819.63745165509</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>45</v>
@@ -9384,15 +9396,15 @@
         <v>325</v>
       </c>
       <c r="AJ97" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AZ97" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="98">
       <c r="A98" s="10">
-        <v>45820.536212800929</v>
+        <v>45820.53621280093</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>45</v>
@@ -9449,15 +9461,15 @@
         <v>325</v>
       </c>
       <c r="AJ98" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ98" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="99">
       <c r="A99" s="8">
-        <v>45820.537087002318</v>
+        <v>45820.53708700232</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>45</v>
@@ -9526,7 +9538,7 @@
         <v>328</v>
       </c>
       <c r="BB99" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC99" s="9" t="s">
         <v>166</v>
@@ -9535,7 +9547,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="100">
       <c r="A100" s="10">
         <v>45820.540335763886</v>
       </c>
@@ -9609,21 +9621,21 @@
         <v>329</v>
       </c>
       <c r="AQ100" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="AY100" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ100" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE100" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="101">
       <c r="A101" s="8">
-        <v>45820.550402731482</v>
+        <v>45820.55040273148</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>45</v>
@@ -9695,19 +9707,19 @@
         <v>334</v>
       </c>
       <c r="AQ101" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AY101" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ101" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BE101" s="9" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="102" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="102">
       <c r="A102" s="10">
         <v>45820.55679234954</v>
       </c>
@@ -9781,7 +9793,7 @@
         <v>183</v>
       </c>
       <c r="BB102" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC102" s="11" t="s">
         <v>69</v>
@@ -9790,9 +9802,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="103">
       <c r="A103" s="8">
-        <v>45820.560375474539</v>
+        <v>45820.56037547454</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>45</v>
@@ -9849,18 +9861,18 @@
         <v>63</v>
       </c>
       <c r="AJ103" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AZ103" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BE103" s="9" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="104" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="104">
       <c r="A104" s="10">
-        <v>45820.568070185182</v>
+        <v>45820.56807018518</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>45</v>
@@ -9932,7 +9944,7 @@
         <v>68</v>
       </c>
       <c r="BB104" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC104" s="11" t="s">
         <v>69</v>
@@ -9941,7 +9953,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="105" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="105">
       <c r="A105" s="8">
         <v>45820.574043252316</v>
       </c>
@@ -10015,21 +10027,21 @@
         <v>241</v>
       </c>
       <c r="AQ105" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AY105" s="9" t="s">
         <v>162</v>
       </c>
       <c r="AZ105" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE105" s="9" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="106" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="106">
       <c r="A106" s="10">
-        <v>45820.576127210647</v>
+        <v>45820.57612721065</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>45</v>
@@ -10098,7 +10110,7 @@
         <v>68</v>
       </c>
       <c r="BB106" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC106" s="11" t="s">
         <v>166</v>
@@ -10107,9 +10119,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="107">
       <c r="A107" s="8">
-        <v>45820.577494409721</v>
+        <v>45820.57749440972</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>45</v>
@@ -10178,7 +10190,7 @@
         <v>68</v>
       </c>
       <c r="BB107" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC107" s="9" t="s">
         <v>166</v>
@@ -10187,7 +10199,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="108" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="108">
       <c r="A108" s="10">
         <v>45820.578042407404</v>
       </c>
@@ -10258,21 +10270,21 @@
         <v>209</v>
       </c>
       <c r="AQ108" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AY108" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ108" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BE108" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="109" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="109">
       <c r="A109" s="8">
-        <v>45820.581439641202</v>
+        <v>45820.5814396412</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>45</v>
@@ -10332,15 +10344,15 @@
         <v>224</v>
       </c>
       <c r="AQ109" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ109" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="110">
       <c r="A110" s="10">
-        <v>45820.597224456018</v>
+        <v>45820.59722445602</v>
       </c>
       <c r="B110" s="11" t="s">
         <v>45</v>
@@ -10412,7 +10424,7 @@
         <v>68</v>
       </c>
       <c r="BB110" s="11">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC110" s="11" t="s">
         <v>229</v>
@@ -10424,9 +10436,9 @@
         <v>346</v>
       </c>
     </row>
-    <row r="111" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="111">
       <c r="A111" s="8">
-        <v>45820.607533043978</v>
+        <v>45820.60753304398</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>45</v>
@@ -10498,7 +10510,7 @@
         <v>68</v>
       </c>
       <c r="BB111" s="9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="BC111" s="9" t="s">
         <v>69</v>
@@ -10510,7 +10522,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="112" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="112">
       <c r="A112" s="10">
         <v>45820.608298136576</v>
       </c>
@@ -10566,10 +10578,10 @@
         <v>350</v>
       </c>
       <c r="AZ112" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="113">
       <c r="A113" s="8">
         <v>45820.620888460646</v>
       </c>
@@ -10640,7 +10652,7 @@
         <v>352</v>
       </c>
       <c r="BB113" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC113" s="9" t="s">
         <v>88</v>
@@ -10649,7 +10661,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="114" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="114">
       <c r="A114" s="10">
         <v>45820.620918298606</v>
       </c>
@@ -10723,16 +10735,16 @@
         <v>241</v>
       </c>
       <c r="AQ114" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AY114" s="11" t="s">
         <v>162</v>
       </c>
       <c r="AZ114" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="115">
       <c r="A115" s="8">
         <v>45820.621696111106</v>
       </c>
@@ -10791,18 +10803,18 @@
         <v>325</v>
       </c>
       <c r="AQ115" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="AZ115" s="9">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BE115" s="9" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="116" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="116">
       <c r="A116" s="10">
-        <v>45820.694278032403</v>
+        <v>45820.6942780324</v>
       </c>
       <c r="B116" s="11" t="s">
         <v>279</v>
@@ -10871,7 +10883,7 @@
         <v>186</v>
       </c>
       <c r="BB116" s="11">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="BC116" s="11" t="s">
         <v>69</v>
@@ -10880,7 +10892,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="117" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="117">
       <c r="A117" s="8">
         <v>45820.746842002314</v>
       </c>
@@ -10951,7 +10963,7 @@
         <v>68</v>
       </c>
       <c r="BB117" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC117" s="9" t="s">
         <v>166</v>
@@ -10960,7 +10972,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="118">
       <c r="A118" s="10">
         <v>45820.760305856486</v>
       </c>
@@ -11019,13 +11031,13 @@
         <v>209</v>
       </c>
       <c r="AJ118" s="11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="AZ118" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="119">
       <c r="A119" s="8">
         <v>45820.881843993055</v>
       </c>
@@ -11099,7 +11111,7 @@
         <v>261</v>
       </c>
       <c r="BB119" s="9">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="BC119" s="9" t="s">
         <v>89</v>
@@ -11108,9 +11120,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="120">
       <c r="A120" s="10">
-        <v>45821.009940960648</v>
+        <v>45821.00994096065</v>
       </c>
       <c r="B120" s="11" t="s">
         <v>45</v>
@@ -11185,7 +11197,7 @@
         <v>360</v>
       </c>
       <c r="BB120" s="11">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="BC120" s="11" t="s">
         <v>361</v>
@@ -11197,9 +11209,9 @@
         <v>362</v>
       </c>
     </row>
-    <row r="121" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="121">
       <c r="A121" s="8">
-        <v>45821.349116192127</v>
+        <v>45821.34911619213</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>45</v>
@@ -11256,87 +11268,691 @@
         <v>209</v>
       </c>
       <c r="AQ121" s="9">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="AZ121" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:57" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="12">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="10">
         <v>45821.35731146991</v>
       </c>
-      <c r="B122" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C122" s="13" t="s">
+      <c r="B122" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C122" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D122" s="13" t="s">
+      <c r="D122" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E122" s="13" t="s">
+      <c r="E122" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J122" s="13" t="s">
+      <c r="J122" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O122" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="P122" s="13" t="s">
+      <c r="O122" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P122" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="R122" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U122" s="13" t="s">
+      <c r="R122" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="U122" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="W122" s="13" t="s">
+      <c r="W122" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="X122" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y122" s="13" t="s">
+      <c r="X122" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y122" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="Z122" s="13" t="s">
+      <c r="Z122" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AA122" s="13" t="s">
+      <c r="AA122" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="AB122" s="13" t="s">
+      <c r="AB122" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AC122" s="13" t="s">
+      <c r="AC122" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AD122" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO122" s="13" t="s">
+      <c r="AD122" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO122" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="AP122" s="13" t="s">
+      <c r="AP122" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="AQ122" s="13">
-        <v>3</v>
-      </c>
-      <c r="AZ122" s="13">
-        <v>4</v>
-      </c>
-      <c r="BE122" s="13" t="s">
+      <c r="AQ122" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="AZ122" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="BE122" s="11" t="s">
         <v>365</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" s="8">
+        <v>45821.488193125</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H123" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="O123" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P123" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="R123" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U123" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W123" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="X123" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y123" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z123" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA123" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB123" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD123" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK123" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL123" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM123" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN123" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="AO123" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP123" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AQ123" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="AY123" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AZ123" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="BE123" s="9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="10">
+        <v>45821.90076722222</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J124" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="O124" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P124" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R124" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="U124" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W124" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="X124" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y124" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z124" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA124" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB124" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC124" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD124" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK124" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL124" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM124" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN124" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY124" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA124" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="BB124" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="BC124" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="BD124" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="8">
+        <v>45822.33873590278</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E125" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J125" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O125" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P125" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q125" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R125" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U125" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W125" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X125" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y125" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z125" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA125" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB125" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD125" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="AI125" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ125" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="AZ125" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="BE125" s="9" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="10">
+        <v>45822.33873858796</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J126" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O126" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P126" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q126" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="R126" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="U126" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W126" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="X126" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y126" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z126" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA126" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB126" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC126" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD126" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="AI126" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ126" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="AZ126" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="BE126" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="8">
+        <v>45822.634392604166</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H127" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="O127" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P127" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R127" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U127" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W127" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="X127" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y127" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z127" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA127" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB127" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD127" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK127" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL127" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM127" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN127" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY127" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA127" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="BB127" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="BC127" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="BD127" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="10">
+        <v>45822.634933124995</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="M128" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="O128" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P128" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R128" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="U128" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W128" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="X128" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y128" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z128" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA128" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB128" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC128" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD128" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK128" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL128" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM128" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN128" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY128" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA128" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="BB128" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="BC128" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD128" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="8">
+        <v>45822.80170386574</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G129" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="M129" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="O129" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P129" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R129" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U129" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W129" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X129" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y129" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z129" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA129" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB129" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD129" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI129" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AJ129" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="AZ129" s="9">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="12">
+        <v>45822.965425601855</v>
+      </c>
+      <c r="B130" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D130" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E130" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J130" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O130" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P130" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="R130" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U130" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="W130" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="X130" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y130" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z130" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA130" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB130" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC130" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD130" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI130" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="AJ130" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="AZ130" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="BE130" s="13" t="s">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>